<commit_message>
Parou de dar o erro doido
</commit_message>
<xml_diff>
--- a/tarefas.xlsx
+++ b/tarefas.xlsx
@@ -437,7 +437,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,6 +481,9 @@
       <c r="B3" s="1">
         <v>42971.902777777781</v>
       </c>
+      <c r="C3" s="1">
+        <v>42971.958333333336</v>
+      </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
@@ -488,6 +491,9 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42973.395833333336</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Tentativa de usar a antTweakBar Primeira etapa é começar a usar render passes para ter acesso à renderização.
</commit_message>
<xml_diff>
--- a/tarefas.xlsx
+++ b/tarefas.xlsx
@@ -116,10 +116,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,13 +438,14 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.77734375" customWidth="1"/>
-    <col min="2" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -495,6 +497,9 @@
       <c r="B4" s="1">
         <v>42973.395833333336</v>
       </c>
+      <c r="C4" s="3">
+        <v>42975.875</v>
+      </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>

</xml_diff>